<commit_message>
Merged with master branch and fixed merging errors
Merged with the updated version in the master branch, and fixing the errors that came out as a result of previous coding style.
</commit_message>
<xml_diff>
--- a/cea/databases/SG/components/FEEDSTOCKS.xlsx
+++ b/cea/databases/SG/components/FEEDSTOCKS.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimathia\Documents\GitHub\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CityEnergyAnalyst\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CD7EDD-1DDE-4835-97E5-C07097DFBF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD3471B-413B-420D-82A3-71A08E512274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="993" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="993" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GRID" sheetId="28" r:id="rId1"/>
     <sheet name="WOOD" sheetId="32" r:id="rId2"/>
     <sheet name="WETBIOMASS" sheetId="33" r:id="rId3"/>
-    <sheet name="DRYBIOMASS" sheetId="34" r:id="rId4"/>
+    <sheet name="DRYBIOMASS" sheetId="37" r:id="rId4"/>
     <sheet name="COAL" sheetId="31" r:id="rId5"/>
     <sheet name="OIL" sheetId="30" r:id="rId6"/>
     <sheet name="NATURALGAS" sheetId="22" r:id="rId7"/>
@@ -148,7 +148,7 @@
     <author>tc={F94F9467-C88C-46C1-8422-4A69C2D3AF2D}</author>
   </authors>
   <commentList>
-    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{F94F9467-C88C-46C1-8422-4A69C2D3AF2D}">
+    <comment ref="I25" authorId="0" shapeId="0" xr:uid="{F94F9467-C88C-46C1-8422-4A69C2D3AF2D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -168,7 +168,7 @@
     <author>Jimeno</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{4825D1AE-8906-4DCD-A08B-1202667547C8}">
       <text>
         <r>
           <rPr>
@@ -181,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{DD0CDEFA-F900-4C10-AC25-4C429A93A60E}">
       <text>
         <r>
           <rPr>
@@ -194,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{AB6042D5-7A88-4D5C-A526-4EE66243BC90}">
       <text>
         <r>
           <rPr>
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="151">
   <si>
     <t>reference</t>
   </si>
@@ -1004,6 +1004,15 @@
   </si>
   <si>
     <t>HYDROGEN</t>
+  </si>
+  <si>
+    <t>Electricity - direct current (low voltage)</t>
+  </si>
+  <si>
+    <t>E30DC</t>
+  </si>
+  <si>
+    <t>DC</t>
   </si>
 </sst>
 </file>
@@ -1680,10 +1689,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I24" dT="2024-04-09T04:55:21.05" personId="{E50E1AEE-1591-4724-8180-022D8812DE3E}" id="{F94F9467-C88C-46C1-8422-4A69C2D3AF2D}">
+  <threadedComment ref="I25" dT="2024-04-09T04:55:21.05" personId="{E50E1AEE-1591-4724-8180-022D8812DE3E}" id="{F94F9467-C88C-46C1-8422-4A69C2D3AF2D}">
     <text>Question by Zhongming: Shall we change all numbers under Tab Solar to 0?</text>
   </threadedComment>
-  <threadedComment ref="I24" dT="2024-04-09T04:56:09.61" personId="{E50E1AEE-1591-4724-8180-022D8812DE3E}" id="{53BA1200-8A82-4429-9BA1-AEC620E5E348}" parentId="{F94F9467-C88C-46C1-8422-4A69C2D3AF2D}">
+  <threadedComment ref="I25" dT="2024-04-09T04:56:09.61" personId="{E50E1AEE-1591-4724-8180-022D8812DE3E}" id="{53BA1200-8A82-4429-9BA1-AEC620E5E348}" parentId="{F94F9467-C88C-46C1-8422-4A69C2D3AF2D}">
     <text>The solar energy here describes actual radiation, while the solar-tab in the original feedstock expresses electricity from photovoltaics. So that does not apply here. So merging the two doesn't make sense, but we could consider differentiating their names a bit more.</text>
   </threadedComment>
 </ThreadedComments>
@@ -1694,19 +1703,19 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1723,457 +1732,409 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C2" s="2">
-        <f>0.24*0.742</f>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D2" s="2">
-        <f>0.24*0.742</f>
-        <v>0.17807999999999999</v>
+      <c r="C2" s="1">
+        <v>0.13150700000000001</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.10520560000000001</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C3" s="2">
-        <f t="shared" ref="C3:D25" si="0">0.24*0.742</f>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D3" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C3" s="1">
+        <v>0.112807</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9.0245600000000009E-2</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C4" s="1">
+        <v>0.10774100000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.6192800000000014E-2</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C5" s="1">
+        <v>0.105602</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8.4481600000000004E-2</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C6" s="1">
+        <v>0.10601600000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>8.4812800000000022E-2</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C7" s="1">
+        <v>0.11487399999999999</v>
+      </c>
+      <c r="D7" s="1">
+        <v>9.18992E-2</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C8" s="1">
+        <v>0.12908699999999998</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.10326959999999999</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C9" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D9" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C9" s="1">
+        <v>0.20460899999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.1636872</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C10" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D10" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C10" s="1">
+        <v>0.26197799999999999</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.2095824</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C11" s="1">
+        <v>0.31157600000000002</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.24926080000000003</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C12" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D12" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C12" s="1">
+        <v>0.33723599999999998</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.2697888</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C13" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D13" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C13" s="1">
+        <v>0.32038800000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.25631039999999999</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C14" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D14" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C14" s="1">
+        <v>0.29694299999999996</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.23755439999999997</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C15" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D15" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C15" s="1">
+        <v>0.32598800000000006</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.26079040000000003</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C16" s="1">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.26640000000000003</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C17" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D17" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C17" s="1">
+        <v>0.35919999999999996</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.28736</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C18" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D18" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C18" s="1">
+        <v>0.34684799999999993</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.27747839999999996</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C19" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C19" s="1">
+        <v>0.31774400000000003</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.25419520000000001</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C20" s="1">
+        <v>0.295298</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.23623840000000002</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C21" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D21" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C21" s="1">
+        <v>0.29566700000000001</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.23653360000000001</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C22" s="1">
+        <v>0.32689799999999991</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.26151839999999993</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C23" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D23" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C23" s="1">
+        <v>0.23178800000000002</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.18543040000000002</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C24" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C24" s="1">
+        <v>0.19042300000000001</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.15233840000000001</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C25" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17807999999999999</v>
+      <c r="C25" s="1">
+        <v>0.14298499999999997</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.11438799999999999</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>59</v>
@@ -2185,9 +2146,6 @@
     <hyperlink ref="E3:E25" r:id="rId2" display="https://www.ema.gov.sg/Residential_Electricity_Tariffs." xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2:A25" numberStoredAsText="1"/>
-  </ignoredErrors>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
@@ -2200,16 +2158,16 @@
       <selection activeCell="D47" sqref="D47:E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -2226,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -2243,7 +2201,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -2260,7 +2218,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -2277,7 +2235,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -2294,7 +2252,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -2311,7 +2269,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -2328,7 +2286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -2345,7 +2303,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -2362,7 +2320,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -2379,7 +2337,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2396,7 +2354,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -2413,7 +2371,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -2430,7 +2388,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -2447,7 +2405,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -2464,7 +2422,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -2481,7 +2439,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
@@ -2498,7 +2456,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -2515,7 +2473,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -2532,7 +2490,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
@@ -2549,7 +2507,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -2566,7 +2524,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -2583,7 +2541,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -2600,7 +2558,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -2617,7 +2575,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
@@ -2642,19 +2600,19 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCBFA07-C74E-3041-BA3F-0C22B6E59680}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="139.36328125" customWidth="1"/>
+    <col min="9" max="9" width="139.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>60</v>
       </c>
@@ -2683,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>67</v>
       </c>
@@ -2710,7 +2668,7 @@
       </c>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>73</v>
       </c>
@@ -2737,7 +2695,7 @@
       </c>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>75</v>
       </c>
@@ -2764,7 +2722,7 @@
       </c>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>77</v>
       </c>
@@ -2791,7 +2749,7 @@
       </c>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>79</v>
       </c>
@@ -2818,7 +2776,7 @@
       </c>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>82</v>
       </c>
@@ -2845,7 +2803,7 @@
       </c>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>85</v>
       </c>
@@ -2872,7 +2830,7 @@
       </c>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>87</v>
       </c>
@@ -2899,7 +2857,7 @@
       </c>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>89</v>
       </c>
@@ -2926,7 +2884,7 @@
       </c>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>91</v>
       </c>
@@ -2953,7 +2911,7 @@
       </c>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>93</v>
       </c>
@@ -2980,18 +2938,18 @@
       </c>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>95</v>
+        <v>148</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>99</v>
@@ -3000,50 +2958,48 @@
         <v>100</v>
       </c>
       <c r="G13" s="23">
+        <v>30</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="23">
         <v>230</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H14" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I14" s="21" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="97" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
+    <row r="15" spans="1:9" ht="96.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B15" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="G14" s="16">
-        <v>22000</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>97</v>
@@ -3051,57 +3007,57 @@
       <c r="D15" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="15" t="s">
         <v>100</v>
       </c>
       <c r="G15" s="16">
-        <v>66000</v>
+        <v>22000</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>139</v>
       </c>
       <c r="I15" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="16">
+        <v>66000</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="I16" s="21" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B17" s="13" t="s">
         <v>109</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>115</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>110</v>
@@ -3119,18 +3075,18 @@
         <v>113</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>110</v>
@@ -3148,24 +3104,24 @@
         <v>113</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>110</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>112</v>
@@ -3177,18 +3133,18 @@
         <v>113</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>110</v>
@@ -3206,18 +3162,18 @@
         <v>113</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>110</v>
@@ -3228,31 +3184,31 @@
       <c r="E21" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="H21" s="16" t="s">
-        <v>145</v>
+      <c r="H21" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>110</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>112</v>
@@ -3264,73 +3220,73 @@
         <v>113</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C23" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D23" s="14" t="s">
         <v>111</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="H23" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>130</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="I24" s="26" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
-        <v>135</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>131</v>
@@ -3345,21 +3301,21 @@
         <v>133</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="G25" s="18">
-        <v>200</v>
+        <v>113</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="I25" s="21" t="s">
+      <c r="I25" s="26" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>131</v>
@@ -3377,7 +3333,7 @@
         <v>136</v>
       </c>
       <c r="G26" s="18">
-        <v>1500</v>
+        <v>200</v>
       </c>
       <c r="H26" s="18" t="s">
         <v>113</v>
@@ -3386,8 +3342,38 @@
         <v>134</v>
       </c>
     </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="G27" s="18">
+        <v>1500</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3397,19 +3383,19 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6328125" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -3426,480 +3412,408 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="9">
-        <f t="shared" ref="B2:B25" si="0">0.027/3.6</f>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" ref="C2:D17" si="1">0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18:D25" si="2">0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="9">
-        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -3908,9 +3822,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2:A25" numberStoredAsText="1"/>
-  </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3920,19 +3831,19 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6328125" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -3949,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -3957,18 +3868,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" ref="C2:D17" si="0">0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -3976,18 +3885,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -3995,18 +3902,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -4014,18 +3919,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -4033,18 +3936,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -4052,18 +3953,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -4071,18 +3970,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -4090,18 +3987,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -4109,18 +4004,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -4128,18 +4021,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -4147,18 +4038,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -4166,18 +4055,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -4185,18 +4072,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -4204,18 +4089,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -4223,18 +4106,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
@@ -4242,18 +4123,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -4261,18 +4140,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18:D25" si="1">0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -4280,18 +4157,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
@@ -4299,18 +4174,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -4318,18 +4191,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -4337,18 +4208,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -4356,18 +4225,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -4375,18 +4242,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
@@ -4394,11 +4259,9 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -4412,23 +4275,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13C13B4-F5EA-4D84-8685-1C88D5FA5F44}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6328125" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -4445,480 +4308,408 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <f>0.027/3.6</f>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" ref="C2:D17" si="0">0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B25" si="1">0.027/3.6</f>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18:D25" si="2">0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="2"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -4936,19 +4727,19 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B25"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6328125" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -4965,7 +4756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -4973,18 +4764,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" ref="C2:D17" si="0">0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -4992,18 +4781,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -5011,18 +4798,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -5030,18 +4815,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -5049,18 +4832,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -5068,18 +4849,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -5087,18 +4866,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -5106,18 +4883,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -5125,18 +4900,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -5144,18 +4917,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -5163,18 +4934,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -5182,18 +4951,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -5201,18 +4968,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -5220,18 +4985,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -5239,18 +5002,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
@@ -5258,18 +5019,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="0"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -5277,18 +5036,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18:D25" si="1">0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -5296,18 +5053,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
@@ -5315,18 +5070,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -5334,18 +5087,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -5353,18 +5104,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -5372,18 +5121,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -5391,18 +5138,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
@@ -5410,11 +5155,9 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -5432,19 +5175,19 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B25"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -5461,7 +5204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -5469,18 +5212,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C2" s="2">
-        <f>0.08*1.04</f>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D2" s="2">
-        <f>0.08*1.04</f>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -5488,18 +5229,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:D25" si="0">0.08*1.04</f>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -5507,18 +5246,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -5526,18 +5263,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -5545,18 +5280,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -5564,18 +5297,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -5583,18 +5314,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -5602,18 +5331,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -5621,18 +5348,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -5640,18 +5365,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -5659,18 +5382,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -5678,18 +5399,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -5697,18 +5416,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -5716,18 +5433,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -5735,18 +5450,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
@@ -5754,18 +5467,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -5773,18 +5484,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -5792,18 +5501,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
@@ -5811,18 +5518,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -5830,18 +5535,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -5849,18 +5552,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -5868,18 +5569,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -5887,18 +5586,16 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
@@ -5906,11 +5603,9 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="0"/>
         <v>8.320000000000001E-2</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -5928,19 +5623,19 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -5957,7 +5652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -5974,7 +5669,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -5991,7 +5686,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -6008,7 +5703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -6025,7 +5720,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -6042,7 +5737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -6059,7 +5754,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -6076,7 +5771,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -6093,7 +5788,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -6110,7 +5805,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -6127,7 +5822,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -6144,7 +5839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -6161,7 +5856,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -6178,7 +5873,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -6195,7 +5890,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -6212,7 +5907,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
@@ -6229,7 +5924,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -6246,7 +5941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -6263,7 +5958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
@@ -6280,7 +5975,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -6297,7 +5992,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -6314,7 +6009,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -6331,7 +6026,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -6348,7 +6043,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
@@ -6378,20 +6073,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -6408,7 +6103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -6425,7 +6120,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -6442,7 +6137,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -6459,7 +6154,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -6476,7 +6171,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -6493,7 +6188,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -6510,7 +6205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -6527,7 +6222,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -6544,7 +6239,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -6561,7 +6256,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -6578,7 +6273,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -6595,7 +6290,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -6612,7 +6307,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -6629,7 +6324,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -6646,7 +6341,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -6663,7 +6358,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
@@ -6680,7 +6375,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -6697,7 +6392,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -6714,7 +6409,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
@@ -6731,7 +6426,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -6748,7 +6443,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -6765,7 +6460,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -6782,7 +6477,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -6799,7 +6494,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
@@ -6833,12 +6528,12 @@
       <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="94.453125" customWidth="1"/>
+    <col min="5" max="5" width="94.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -6855,7 +6550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -6872,7 +6567,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -6889,7 +6584,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -6906,7 +6601,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -6923,7 +6618,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -6940,7 +6635,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -6957,7 +6652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -6974,7 +6669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -6991,7 +6686,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -7008,7 +6703,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -7025,7 +6720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -7042,7 +6737,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -7059,7 +6754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -7076,7 +6771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -7093,7 +6788,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -7110,7 +6805,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
@@ -7127,7 +6822,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -7144,7 +6839,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -7161,7 +6856,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
@@ -7178,7 +6873,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -7195,7 +6890,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -7212,7 +6907,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -7229,7 +6924,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -7246,7 +6941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>

</xml_diff>